<commit_message>
Fertig v7 für Uni
</commit_message>
<xml_diff>
--- a/Backend/R2_Simulink_full.xlsx
+++ b/Backend/R2_Simulink_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taras\Documents\HAW\Batterietechnik_Studienarbeit\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D3E77F-B51C-41C0-9E20-3F6B02847661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075A4A31-C4DD-4499-91AE-79ECAF5EEC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5637580-7A38-42BB-AD33-11071E515969}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DE05DC07-BF2C-4EAA-837F-5A4FE95854AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Time</t>
+    <t>Zeit_sim [s]</t>
   </si>
   <si>
-    <t>R2</t>
+    <t>R2_sim_full [Ohm]</t>
   </si>
 </sst>
 </file>
@@ -392,14 +392,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C697FD-977D-42EC-8F84-CE58692F61D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE42B0F-87DE-42AA-BC60-811D8B2B3828}">
   <dimension ref="A1:B2362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2362"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7790,7 +7793,7 @@
         <v>461</v>
       </c>
       <c r="B924">
-        <v>1.1384139529786699E-3</v>
+        <v>1.13841395297866E-3</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.25">
@@ -7878,7 +7881,7 @@
         <v>466.5</v>
       </c>
       <c r="B935">
-        <v>1.1420761486790299E-3</v>
+        <v>1.1420761486790199E-3</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.25">
@@ -9086,7 +9089,7 @@
         <v>542</v>
       </c>
       <c r="B1086">
-        <v>1.2501981628559799E-3</v>
+        <v>1.2501981628559699E-3</v>
       </c>
     </row>
     <row r="1087" spans="1:2" x14ac:dyDescent="0.25">
@@ -11334,7 +11337,7 @@
         <v>682.5</v>
       </c>
       <c r="B1367">
-        <v>1.04348493513054E-3</v>
+        <v>1.04348493513053E-3</v>
       </c>
     </row>
     <row r="1368" spans="1:2" x14ac:dyDescent="0.25">
@@ -11494,7 +11497,7 @@
         <v>692.5</v>
       </c>
       <c r="B1387">
-        <v>1.0520743835981301E-3</v>
+        <v>1.0520743835981199E-3</v>
       </c>
     </row>
     <row r="1388" spans="1:2" x14ac:dyDescent="0.25">
@@ -11646,7 +11649,7 @@
         <v>702</v>
       </c>
       <c r="B1406">
-        <v>1.06061186671475E-3</v>
+        <v>1.0606118667147401E-3</v>
       </c>
     </row>
     <row r="1407" spans="1:2" x14ac:dyDescent="0.25">
@@ -12134,7 +12137,7 @@
         <v>732.5</v>
       </c>
       <c r="B1467">
-        <v>1.23678721772309E-3</v>
+        <v>1.2367872177231E-3</v>
       </c>
     </row>
     <row r="1468" spans="1:2" x14ac:dyDescent="0.25">
@@ -14798,7 +14801,7 @@
         <v>899</v>
       </c>
       <c r="B1800">
-        <v>1.18541496035799E-3</v>
+        <v>1.1854149603579801E-3</v>
       </c>
     </row>
     <row r="1801" spans="1:2" x14ac:dyDescent="0.25">
@@ -18582,7 +18585,7 @@
         <v>1135.5</v>
       </c>
       <c r="B2273">
-        <v>1.29318160027359E-3</v>
+        <v>1.2931816002735999E-3</v>
       </c>
     </row>
     <row r="2274" spans="1:2" x14ac:dyDescent="0.25">
@@ -18598,7 +18601,7 @@
         <v>1136.5</v>
       </c>
       <c r="B2275">
-        <v>1.27472793078659E-3</v>
+        <v>1.2747279307865999E-3</v>
       </c>
     </row>
     <row r="2276" spans="1:2" x14ac:dyDescent="0.25">
@@ -18606,7 +18609,7 @@
         <v>1137</v>
       </c>
       <c r="B2276">
-        <v>1.2646448646619699E-3</v>
+        <v>1.2646448646619799E-3</v>
       </c>
     </row>
     <row r="2277" spans="1:2" x14ac:dyDescent="0.25">
@@ -18622,7 +18625,7 @@
         <v>1138</v>
       </c>
       <c r="B2278">
-        <v>1.2496719447323201E-3</v>
+        <v>1.2496719447323301E-3</v>
       </c>
     </row>
     <row r="2279" spans="1:2" x14ac:dyDescent="0.25">
@@ -18806,7 +18809,7 @@
         <v>1149.5</v>
       </c>
       <c r="B2301">
-        <v>9.9178196147763596E-4</v>
+        <v>9.9178196147763509E-4</v>
       </c>
     </row>
     <row r="2302" spans="1:2" x14ac:dyDescent="0.25">
@@ -18902,7 +18905,7 @@
         <v>1155.5</v>
       </c>
       <c r="B2313">
-        <v>1.05282425254322E-3</v>
+        <v>1.05282425254321E-3</v>
       </c>
     </row>
     <row r="2314" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>